<commit_message>
run_this.py needs to be optimized
</commit_message>
<xml_diff>
--- a/case/testcase.xlsx
+++ b/case/testcase.xlsx
@@ -1,152 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bear\PycharmProjects\ReportApiTest01\case\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362B2857-74B0-48DE-8C58-EB6D5E8DE226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9B234BDB-7E62-4D63-B834-2F67555BAF06}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="p1" sheetId="1" r:id="rId1"/>
+    <sheet name="p1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>case_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>model_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>case_title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>method</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>payload</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>expect_result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>actual_result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>test_result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/datack/Collect/CollectList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>效率总览</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-    "lineNo": 1,
-    "sideNo": 1,
-    "tagsContains": [
-        "TAG_IV_TEST=实验批次"
-    ],
-    "tagsNotContains": [
-        "TAG_IV_TEST=实验批次"
-    ]
-}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>headers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,47 +102,107 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -522,86 +502,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A806632-DA55-4A9D-88C8-09240A92EBF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.21875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="7" width="34.44140625" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col width="12.21875" customWidth="1" style="6" min="1" max="1"/>
+    <col width="32.33203125" customWidth="1" style="6" min="2" max="2"/>
+    <col width="25.109375" customWidth="1" style="6" min="3" max="3"/>
+    <col width="20.109375" customWidth="1" style="6" min="4" max="4"/>
+    <col width="18.6640625" customWidth="1" style="6" min="5" max="5"/>
+    <col width="34.44140625" customWidth="1" style="6" min="6" max="7"/>
+    <col width="18.33203125" customWidth="1" style="6" min="8" max="8"/>
+    <col width="17" customWidth="1" style="6" min="9" max="9"/>
+    <col width="13.77734375" customWidth="1" style="6" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="17.4" customHeight="1" s="6">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>case_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>model_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>case_title</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>payload</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>headers</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>expect_result</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>actual_result</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>test_result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="138" customHeight="1" s="6">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>效率总览</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>/datack/Collect/CollectList</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>效率总览</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>{
+    "lineNo": 1,
+    "sideNo": 1,
+    "tagsContains": [
+        "TAG_IV_TEST=实验批次"
+    ],
+    "tagsNotContains": [
+        "TAG_IV_TEST=实验批次"
+    ]
+}</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
basic frame was down--version1.0 to be optimized: testlog.log / testcase
</commit_message>
<xml_diff>
--- a/case/testcase.xlsx
+++ b/case/testcase.xlsx
@@ -1,160 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bear\PycharmProjects\ReportApiTest01\case\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AEABBB-54EE-4CB7-BDD1-594B264F1928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="p1" sheetId="1" r:id="rId1"/>
+    <sheet name="p1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
-  <si>
-    <t>case_id</t>
-  </si>
-  <si>
-    <t>model_name</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>case_title</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>payload</t>
-  </si>
-  <si>
-    <t>headers</t>
-  </si>
-  <si>
-    <t>expect_result</t>
-  </si>
-  <si>
-    <t>actual_result</t>
-  </si>
-  <si>
-    <t>test_result</t>
-  </si>
-  <si>
-    <t>效率总览</t>
-  </si>
-  <si>
-    <t>/datack/Collect/CollectList</t>
-  </si>
-  <si>
-    <t>post</t>
-  </si>
-  <si>
-    <t>{
-    "lineNo": 1,
-    "sideNo": 1,
-    "tagsContains": [
-        "TAG_IV_TEST=实验批次"
-    ],
-    "tagsNotContains": [
-        "TAG_IV_TEST=实验批次"
-    ]
-}</t>
-  </si>
-  <si>
-    <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
-  </si>
-  <si>
-    <t>产量总览（测试）</t>
-  </si>
-  <si>
-    <t>/data-api/1/yield-overview-test</t>
-  </si>
-  <si>
-    <t>{
-    "lineId": 0,
-    "lineNo": 0,
-    "begin": "2024-07-21 00:00:00.000",
-    "end": "2024-08-20 00:00:00.000"
-}</t>
-  </si>
-  <si>
-    <t>产量总览（印刷）</t>
-  </si>
-  <si>
-    <t>/data-api/0/yield-overview-printing</t>
-  </si>
-  <si>
-    <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="3"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -190,48 +102,107 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -531,144 +502,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="6" customWidth="1"/>
-    <col min="6" max="7" width="34.44140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17" style="6" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" style="6" customWidth="1"/>
+    <col width="12.21875" customWidth="1" style="6" min="1" max="1"/>
+    <col width="32.33203125" customWidth="1" style="6" min="2" max="2"/>
+    <col width="25.109375" customWidth="1" style="6" min="3" max="3"/>
+    <col width="20.109375" customWidth="1" style="6" min="4" max="4"/>
+    <col width="18.6640625" customWidth="1" style="6" min="5" max="5"/>
+    <col width="34.44140625" customWidth="1" style="6" min="6" max="7"/>
+    <col width="18.33203125" customWidth="1" style="6" min="8" max="8"/>
+    <col width="17" customWidth="1" style="6" min="9" max="9"/>
+    <col width="13.77734375" customWidth="1" style="6" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" ht="17.4" customHeight="1" s="6">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>case_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>case_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>case_title</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>method</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>payload</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>headers</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>expect_result</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>actual_result</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>test_result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="138" customHeight="1" s="6">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>效率总览</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>/datack/Collect/CollectList</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>效率总览</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+      <c r="F2" s="4" t="inlineStr">
+        <is>
+          <t>{
+    "lineNo": 1,
+    "sideNo": 1,
+    "tagsContains": [
+        "TAG_IV_TEST=实验批次"
+    ],
+    "tagsNotContains": [
+        "TAG_IV_TEST=实验批次"
+    ]
+}</t>
+        </is>
+      </c>
+      <c r="G2" s="4" t="inlineStr">
+        <is>
+          <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
+        </is>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="J2" s="4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="138" customHeight="1" s="6">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>产量总览（测试）</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>/data-api/1/yield-overview-test</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="inlineStr">
+        <is>
+          <t>产量总览（测试）</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="inlineStr">
+        <is>
+          <t>{
+    "lineId": 0,
+    "lineNo": 0,
+    "begin": "2024-07-21 00:00:00.000",
+    "end": "2024-08-20 00:00:00.000"
+}</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="inlineStr">
+        <is>
+          <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="I3" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="J3" s="4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="138" customHeight="1" s="6">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>产量总览（印刷）</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>/data-api/0/yield-overview-printing</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>产量总览（印刷）</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>post</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
+          <t>{
+    "lineId": 0,
+    "lineNo": 0,
+    "begin": "2024-07-21 00:00:00.000",
+    "end": "2024-08-20 00:00:00.000"
+}</t>
+        </is>
+      </c>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>{   "Content-Type": "application/json;charset=UTF-8"          }</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="I4" s="4" t="n">
         <v>200</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4">
-        <v>200</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="inlineStr">
+        <is>
+          <t>pass</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>